<commit_message>
Squash 2 commits: add help tab + reset last change name
Reset the last change name into both xls

New Help Tab

The help tab was missing in the Application and Configuration excel
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
+++ b/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18379018-0DEA-D645-A22B-84E83694A525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E100A21-2BEA-405D-8181-D5129627D273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library Elements" sheetId="1" r:id="rId1"/>
     <sheet name="Element Types" sheetId="2" r:id="rId2"/>
+    <sheet name="Help Portal" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Library Elements'!$A$1:$H$2</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -85,13 +86,16 @@
   </si>
   <si>
     <t>Available Element Types</t>
+  </si>
+  <si>
+    <t>For detailed information on the creation of documents via spreadsheet, see SAP Help Portal.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +138,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF7F7F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,11 +176,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -184,10 +204,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{231B5AA4-E425-4500-8FF9-7AAA09BB6E97}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{FCBB1A3E-82AA-44BC-9F4B-CB2C697C5515}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -514,7 +540,7 @@
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="42.5" style="3" customWidth="1"/>
     <col min="2" max="3" width="20.6640625" style="3" customWidth="1"/>
@@ -528,7 +554,7 @@
     <col min="11" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:67" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -601,7 +627,7 @@
       <c r="AX1" s="3"/>
       <c r="AY1" s="3"/>
     </row>
-    <row r="2" spans="1:67" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -622,7 +648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -639,7 +665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.35">
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
@@ -697,38 +723,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D951F67C-C3F3-774D-9A72-A56DB65E3F99}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -736,4 +762,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADDEE3D-7C9E-4B61-AE3A-717B8AE14B28}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A4:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="10.6640625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:H4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="SAP Help Portal." xr:uid="{0FDD18E3-6F75-4251-A3C4-78178F7B50D7}"/>
+    <hyperlink ref="A4:H4" r:id="rId2" display="For detailed information on the creation of documents via spreadsheet, see SAP Help Portal." xr:uid="{2D2301FA-D938-4BD1-BC9C-01C466ABA383}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add External URL and Name to Excels
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
+++ b/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E100A21-2BEA-405D-8181-D5129627D273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C77A6E-1FB0-425F-A53F-01A43DD397E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65955" yWindow="2610" windowWidth="25935" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library Elements" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>For detailed information on the creation of documents via spreadsheet, see SAP Help Portal.</t>
+  </si>
+  <si>
+    <t>External URL</t>
+  </si>
+  <si>
+    <t>External Name</t>
   </si>
 </sst>
 </file>
@@ -535,26 +541,28 @@
   </sheetPr>
   <dimension ref="A1:BO11"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="42.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="42.47265625" style="3" customWidth="1"/>
     <col min="2" max="3" width="20.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.47265625" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.80859375" style="3" customWidth="1"/>
     <col min="7" max="7" width="27" style="3" customWidth="1"/>
     <col min="8" max="8" width="32" style="3" customWidth="1"/>
-    <col min="9" max="9" width="47.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="47.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="3"/>
+    <col min="11" max="11" width="13.5234375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.80859375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -585,8 +593,12 @@
       <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -627,7 +639,7 @@
       <c r="AX1" s="3"/>
       <c r="AY1" s="3"/>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -648,7 +660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -665,7 +677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.6">
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
@@ -727,34 +739,34 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="26.80859375" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="16384" width="10.80859375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -771,16 +783,16 @@
   </sheetPr>
   <dimension ref="A4:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="16384" width="10.6640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A4" s="12" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Update spreadsheet library templates
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
+++ b/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C77A6E-1FB0-425F-A53F-01A43DD397E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B1009-316C-46ED-A79E-5E110581296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65955" yWindow="2610" windowWidth="25935" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library Elements" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Library Elements'!$A$1:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -101,19 +114,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -153,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -184,34 +196,31 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -542,61 +551,61 @@
   <dimension ref="A1:BO11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="42.47265625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="33.47265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.80859375" style="3" customWidth="1"/>
     <col min="7" max="7" width="27" style="3" customWidth="1"/>
     <col min="8" max="8" width="32" style="3" customWidth="1"/>
-    <col min="9" max="9" width="47.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="47.09375" style="3" customWidth="1"/>
     <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.5234375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.47265625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.90234375" style="3" customWidth="1"/>
     <col min="13" max="16384" width="8.80859375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="2" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="3"/>
@@ -640,20 +649,20 @@
       <c r="AY1" s="3"/>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -664,13 +673,13 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="9" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="7" t="s">
@@ -678,47 +687,47 @@
       </c>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.6">
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="2"/>
-      <c r="AM11" s="2"/>
-      <c r="AN11" s="2"/>
-      <c r="AO11" s="2"/>
-      <c r="AP11" s="2"/>
-      <c r="AQ11" s="2"/>
-      <c r="AR11" s="2"/>
-      <c r="AS11" s="2"/>
-      <c r="AT11" s="2"/>
-      <c r="AU11" s="2"/>
-      <c r="AV11" s="2"/>
-      <c r="AW11" s="2"/>
-      <c r="AX11" s="2"/>
-      <c r="AY11" s="2"/>
-      <c r="AZ11" s="2"/>
-      <c r="BA11" s="2"/>
-      <c r="BB11" s="2"/>
-      <c r="BC11" s="2"/>
-      <c r="BD11" s="2"/>
-      <c r="BE11" s="2"/>
-      <c r="BF11" s="2"/>
-      <c r="BG11" s="2"/>
-      <c r="BH11" s="2"/>
-      <c r="BI11" s="2"/>
-      <c r="BJ11" s="2"/>
-      <c r="BK11" s="2"/>
-      <c r="BL11" s="2"/>
-      <c r="BM11" s="2"/>
-      <c r="BN11" s="2"/>
-      <c r="BO11" s="2"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+      <c r="BJ11" s="1"/>
+      <c r="BK11" s="1"/>
+      <c r="BL11" s="1"/>
+      <c r="BM11" s="1"/>
+      <c r="BN11" s="1"/>
+      <c r="BO11" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -728,6 +737,18 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose Element Type" xr:uid="{218EA752-80E3-42BB-AD98-790399E3BBA1}">
+          <x14:formula1>
+            <xm:f>'Element Types'!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -736,42 +757,45 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="26.80859375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.80859375" style="3"/>
+    <col min="1" max="1" width="26.80859375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.80859375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A2" s="10" t="s">
-        <v>20</v>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A5">
+    <sortCondition ref="A2:A5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -783,26 +807,24 @@
   </sheetPr>
   <dimension ref="A4:H4"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="11"/>
+    <col min="1" max="16384" width="10.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update spreadsheet library templates (#48)
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
+++ b/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C77A6E-1FB0-425F-A53F-01A43DD397E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B1009-316C-46ED-A79E-5E110581296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65955" yWindow="2610" windowWidth="25935" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library Elements" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Library Elements'!$A$1:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -101,19 +114,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -153,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -184,34 +196,31 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -542,61 +551,61 @@
   <dimension ref="A1:BO11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="42.47265625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="33.47265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.80859375" style="3" customWidth="1"/>
     <col min="7" max="7" width="27" style="3" customWidth="1"/>
     <col min="8" max="8" width="32" style="3" customWidth="1"/>
-    <col min="9" max="9" width="47.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="47.09375" style="3" customWidth="1"/>
     <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.5234375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.47265625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.90234375" style="3" customWidth="1"/>
     <col min="13" max="16384" width="8.80859375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="2" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>24</v>
       </c>
       <c r="M1" s="3"/>
@@ -640,20 +649,20 @@
       <c r="AY1" s="3"/>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -664,13 +673,13 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="9" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="7" t="s">
@@ -678,47 +687,47 @@
       </c>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.6">
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="2"/>
-      <c r="AM11" s="2"/>
-      <c r="AN11" s="2"/>
-      <c r="AO11" s="2"/>
-      <c r="AP11" s="2"/>
-      <c r="AQ11" s="2"/>
-      <c r="AR11" s="2"/>
-      <c r="AS11" s="2"/>
-      <c r="AT11" s="2"/>
-      <c r="AU11" s="2"/>
-      <c r="AV11" s="2"/>
-      <c r="AW11" s="2"/>
-      <c r="AX11" s="2"/>
-      <c r="AY11" s="2"/>
-      <c r="AZ11" s="2"/>
-      <c r="BA11" s="2"/>
-      <c r="BB11" s="2"/>
-      <c r="BC11" s="2"/>
-      <c r="BD11" s="2"/>
-      <c r="BE11" s="2"/>
-      <c r="BF11" s="2"/>
-      <c r="BG11" s="2"/>
-      <c r="BH11" s="2"/>
-      <c r="BI11" s="2"/>
-      <c r="BJ11" s="2"/>
-      <c r="BK11" s="2"/>
-      <c r="BL11" s="2"/>
-      <c r="BM11" s="2"/>
-      <c r="BN11" s="2"/>
-      <c r="BO11" s="2"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+      <c r="BJ11" s="1"/>
+      <c r="BK11" s="1"/>
+      <c r="BL11" s="1"/>
+      <c r="BM11" s="1"/>
+      <c r="BN11" s="1"/>
+      <c r="BO11" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -728,6 +737,18 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose Element Type" xr:uid="{218EA752-80E3-42BB-AD98-790399E3BBA1}">
+          <x14:formula1>
+            <xm:f>'Element Types'!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -736,42 +757,45 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="26.80859375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.80859375" style="3"/>
+    <col min="1" max="1" width="26.80859375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.80859375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A2" s="10" t="s">
-        <v>20</v>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A5">
+    <sortCondition ref="A2:A5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -783,26 +807,24 @@
   </sheetPr>
   <dimension ref="A4:H4"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="16384" width="10.6640625" style="11"/>
+    <col min="1" max="16384" width="10.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Excel Templates for SAP Cloud ALM Library Elements
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
+++ b/spreadsheet-examples/spreadsheet-libraries/SAP Cloud ALM - Library Elements Template for Application.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B1009-316C-46ED-A79E-5E110581296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3F14B2-247C-4214-84B3-8E1C9481D656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library Elements" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Help Portal" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Library Elements'!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Library Elements'!$A$1:$M$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +32,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{43CB6A87-9321-4066-9C80-F8ECD78D9A15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mandatory</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{6521C0B4-EA80-4D8C-B29B-6F9BCA41D3A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mandatory</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Title</t>
   </si>
@@ -98,9 +174,6 @@
     <t>SAP Fiori Application</t>
   </si>
   <si>
-    <t>Available Element Types</t>
-  </si>
-  <si>
     <t>For detailed information on the creation of documents via spreadsheet, see SAP Help Portal.</t>
   </si>
   <si>
@@ -108,25 +181,24 @@
   </si>
   <si>
     <t>External Name</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Element Types</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -158,6 +230,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -180,7 +271,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,14 +287,12 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -215,12 +304,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -544,199 +634,207 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BO11"/>
+  <dimension ref="A1:BP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="42.47265625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.47265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="24.80859375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27" style="3" customWidth="1"/>
-    <col min="8" max="8" width="32" style="3" customWidth="1"/>
-    <col min="9" max="9" width="47.09375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.47265625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="14.90234375" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="8.80859375" style="3"/>
+    <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.09375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.80859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.94921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.80859375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:68" s="8" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.6">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.6">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="J3" s="5"/>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.6">
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
-      <c r="AM11" s="1"/>
-      <c r="AN11" s="1"/>
-      <c r="AO11" s="1"/>
-      <c r="AP11" s="1"/>
-      <c r="AQ11" s="1"/>
-      <c r="AR11" s="1"/>
-      <c r="AS11" s="1"/>
-      <c r="AT11" s="1"/>
-      <c r="AU11" s="1"/>
-      <c r="AV11" s="1"/>
-      <c r="AW11" s="1"/>
-      <c r="AX11" s="1"/>
-      <c r="AY11" s="1"/>
-      <c r="AZ11" s="1"/>
-      <c r="BA11" s="1"/>
-      <c r="BB11" s="1"/>
-      <c r="BC11" s="1"/>
-      <c r="BD11" s="1"/>
-      <c r="BE11" s="1"/>
-      <c r="BF11" s="1"/>
-      <c r="BG11" s="1"/>
-      <c r="BH11" s="1"/>
-      <c r="BI11" s="1"/>
-      <c r="BJ11" s="1"/>
-      <c r="BK11" s="1"/>
-      <c r="BL11" s="1"/>
-      <c r="BM11" s="1"/>
-      <c r="BN11" s="1"/>
-      <c r="BO11" s="1"/>
+    <row r="11" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
+      <c r="AM11" s="8"/>
+      <c r="AN11" s="8"/>
+      <c r="AO11" s="8"/>
+      <c r="AP11" s="8"/>
+      <c r="AQ11" s="8"/>
+      <c r="AR11" s="8"/>
+      <c r="AS11" s="8"/>
+      <c r="AT11" s="8"/>
+      <c r="AU11" s="8"/>
+      <c r="AV11" s="8"/>
+      <c r="AW11" s="8"/>
+      <c r="AX11" s="8"/>
+      <c r="AY11" s="8"/>
+      <c r="AZ11" s="8"/>
+      <c r="BA11" s="8"/>
+      <c r="BB11" s="8"/>
+      <c r="BC11" s="8"/>
+      <c r="BD11" s="8"/>
+      <c r="BE11" s="8"/>
+      <c r="BF11" s="8"/>
+      <c r="BG11" s="8"/>
+      <c r="BH11" s="8"/>
+      <c r="BI11" s="8"/>
+      <c r="BJ11" s="8"/>
+      <c r="BK11" s="8"/>
+      <c r="BL11" s="8"/>
+      <c r="BM11" s="8"/>
+      <c r="BN11" s="8"/>
+      <c r="BO11" s="8"/>
+      <c r="BP11" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{5B726951-0870-D443-B627-082353F706C6}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{17C6F449-0C5C-C14D-87D0-3AC320661E77}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -756,39 +854,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D951F67C-C3F3-774D-9A72-A56DB65E3F99}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.80859375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="26.80859375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.80859375" style="2"/>
+    <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.80859375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
+      <c r="A1" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -807,24 +903,24 @@
   </sheetPr>
   <dimension ref="A4:H4"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="4"/>
+    <col min="1" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="A4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -836,4 +932,10 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{0cf7ac0a-4681-4823-ab0b-04ef02c5f873}" enabled="1" method="Standard" siteId="{42f7676c-f455-423c-82f6-dc2d99791af7}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>